<commit_message>
Avoid double group label
</commit_message>
<xml_diff>
--- a/doc/Zulassung/students.xlsx
+++ b/doc/Zulassung/students.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/werne/Development/osg-exam/doc/Zulassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F21061D-9E63-174B-BE6E-E3B06C38010A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367AC165-6564-7E49-A248-5D3B2F2EEF08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <r>
       <rPr>
@@ -74,37 +74,6 @@
   <si>
     <r>
       <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Gruppe</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>M_AE</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>M_AI</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
         <sz val="11"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -126,12 +95,6 @@
   </si>
   <si>
     <t>Müstermänn</t>
-  </si>
-  <si>
-    <t>Prüfung</t>
-  </si>
-  <si>
-    <t>Semester</t>
   </si>
   <si>
     <t>MatrikelNUmmer</t>
@@ -235,34 +198,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -569,125 +532,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H134"/>
+  <dimension ref="A1:G134"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.3984375" customWidth="1"/>
-    <col min="2" max="2" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.796875" customWidth="1"/>
-    <col min="5" max="5" width="24.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.796875" customWidth="1"/>
+    <col min="4" max="4" width="24.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="3" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="4" spans="1:8" ht="23" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5">
         <v>20</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>4</v>
+      <c r="B4" s="7">
+        <v>2013</v>
       </c>
       <c r="C4" s="7">
-        <v>2013</v>
-      </c>
-      <c r="D4" s="7">
         <v>4612135</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>20</v>
+      <c r="D4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5">
         <v>44</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>5</v>
+      <c r="B5" s="7">
+        <v>2014</v>
       </c>
       <c r="C5" s="7">
-        <v>2014</v>
-      </c>
-      <c r="D5" s="7">
         <v>4562263</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>21</v>
+      <c r="D5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="7" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="8" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="9" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="10" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="11" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="12" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="13" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="7" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="8" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="9" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="10" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="17" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="18" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="19" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -807,8 +754,8 @@
     <row r="133" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="134" ht="21" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:R134">
-    <sortCondition ref="D4:D134"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:Q134">
+    <sortCondition ref="C4:C134"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -839,7 +786,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>